<commit_message>
Almost finished section 2 report
</commit_message>
<xml_diff>
--- a/Documentation and Final Report/GUDE Usability Test Results.xlsx
+++ b/Documentation and Final Report/GUDE Usability Test Results.xlsx
@@ -171,12 +171,12 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="30.57"/>
-    <col customWidth="1" min="2" max="2" width="34.57"/>
-    <col customWidth="1" min="3" max="3" width="34.86"/>
-    <col customWidth="1" min="4" max="4" width="16.43"/>
-    <col customWidth="1" min="5" max="5" width="29.43"/>
-    <col customWidth="1" min="6" max="6" width="27.43"/>
+    <col customWidth="1" min="1" max="1" width="19.14"/>
+    <col customWidth="1" min="2" max="2" width="30.29"/>
+    <col customWidth="1" min="3" max="3" width="16.86"/>
+    <col customWidth="1" min="4" max="4" width="30.0"/>
+    <col customWidth="1" min="5" max="5" width="27.29"/>
+    <col customWidth="1" min="6" max="6" width="25.0"/>
     <col customWidth="1" min="7" max="7" width="34.14"/>
   </cols>
   <sheetData>
@@ -484,48 +484,48 @@
         <v>21</v>
       </c>
     </row>
+    <row r="24">
+      <c r="A24" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
     <row r="25">
       <c r="A25" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="2" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>